<commit_message>
modified UOM and complete Subset
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/UOMModuleTest.xlsx
+++ b/resources/ExcelsheetData/UOMModuleTest.xlsx
@@ -4,24 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="tc_UOM_001" sheetId="1" r:id="rId1"/>
     <sheet name="tc_UOM_002" sheetId="2" r:id="rId2"/>
-    <sheet name="tc_UOM_004" sheetId="3" r:id="rId3"/>
-    <sheet name="tc_UOM_006" sheetId="4" r:id="rId4"/>
-    <sheet name="tc_UOM_008" sheetId="6" r:id="rId5"/>
-    <sheet name="tc_UOM_003_007" sheetId="8" r:id="rId6"/>
-    <sheet name="tc_UOM_009" sheetId="7" r:id="rId7"/>
-    <sheet name="tc_UOM_005_010" sheetId="9" r:id="rId8"/>
+    <sheet name="tc_UOM_006" sheetId="4" r:id="rId3"/>
+    <sheet name="tc_UOM_008" sheetId="6" r:id="rId4"/>
+    <sheet name="tc_UOM_003_007" sheetId="8" r:id="rId5"/>
+    <sheet name="tc_UOM_004_005_010" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>testCaseId</t>
   </si>
@@ -65,9 +63,6 @@
     <t>UOM Name</t>
   </si>
   <si>
-    <t>AutomationTestUOM</t>
-  </si>
-  <si>
     <t>TC_UOM_006</t>
   </si>
   <si>
@@ -137,9 +132,6 @@
     <t>New Unit Of Measure saved Successfully</t>
   </si>
   <si>
-    <t>TC_UOM_004</t>
-  </si>
-  <si>
     <t>TC_UOM_005</t>
   </si>
   <si>
@@ -152,16 +144,13 @@
     <t>TC_UOM_003_007</t>
   </si>
   <si>
-    <t>TC_UOM_009</t>
-  </si>
-  <si>
     <t>TestAutomation</t>
   </si>
   <si>
-    <t>AutomationQW</t>
-  </si>
-  <si>
-    <t>AutomationUpUOM4</t>
+    <t>Pauto</t>
+  </si>
+  <si>
+    <t>PAutoTest2</t>
   </si>
 </sst>
 </file>
@@ -634,50 +623,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -696,7 +641,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -725,27 +670,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -754,7 +699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -775,48 +720,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -824,57 +769,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,62 +783,69 @@
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>40</v>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated UOM as per review comments
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/UOMModuleTest.xlsx
+++ b/resources/ExcelsheetData/UOMModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="tc_UOM_001" sheetId="1" r:id="rId1"/>
@@ -12,16 +12,15 @@
     <sheet name="tc_UOM_004" sheetId="3" r:id="rId3"/>
     <sheet name="tc_UOM_006" sheetId="4" r:id="rId4"/>
     <sheet name="tc_UOM_008" sheetId="6" r:id="rId5"/>
-    <sheet name="tc_UOM_003_007" sheetId="8" r:id="rId6"/>
-    <sheet name="tc_UOM_009" sheetId="7" r:id="rId7"/>
-    <sheet name="tc_UOM_005_010" sheetId="9" r:id="rId8"/>
+    <sheet name="tc_UOM_009" sheetId="7" r:id="rId6"/>
+    <sheet name="tc_UOM_3_4_5_7_9_10" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>testCaseId</t>
   </si>
@@ -107,30 +106,12 @@
     <t>TestCase ID</t>
   </si>
   <si>
-    <t>User name</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Welcome message</t>
-  </si>
-  <si>
     <t>UOM Description</t>
   </si>
   <si>
     <t>UOM Success Message</t>
   </si>
   <si>
-    <t>automationUser</t>
-  </si>
-  <si>
-    <t>unilog123##</t>
-  </si>
-  <si>
-    <t>Welcome, Automation !</t>
-  </si>
-  <si>
     <t>Created for Automation Test Purpose, Please do not edit or delete by manually.</t>
   </si>
   <si>
@@ -149,19 +130,13 @@
     <t>updated Welcome Message</t>
   </si>
   <si>
-    <t>TC_UOM_003_007</t>
-  </si>
-  <si>
     <t>TC_UOM_009</t>
   </si>
   <si>
-    <t>AutomationTe</t>
-  </si>
-  <si>
-    <t>AutomationTeUOMU</t>
-  </si>
-  <si>
-    <t>AutomationTestUOMUpted5</t>
+    <t>AutomationPR</t>
+  </si>
+  <si>
+    <t>AutomationPR Updated</t>
   </si>
 </sst>
 </file>
@@ -231,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -242,8 +217,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,7 +637,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
@@ -755,76 +731,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -855,7 +761,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
@@ -869,12 +775,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,13 +789,14 @@
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -897,47 +804,53 @@
         <v>13</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>46</v>
+      <c r="E2" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated testng.xml and UOM test data
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/UOMModuleTest.xlsx
+++ b/resources/ExcelsheetData/UOMModuleTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
@@ -15,7 +15,7 @@
     <sheet name="tc_UOM_009" sheetId="7" r:id="rId6"/>
     <sheet name="tc_UOM_3_4_5_7_9_10" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -133,17 +133,17 @@
     <t>TC_UOM_009</t>
   </si>
   <si>
-    <t>AutomationPR</t>
-  </si>
-  <si>
-    <t>AutomationPR Updated</t>
+    <t>AutomationPQR</t>
+  </si>
+  <si>
+    <t>AutomationPQR Updated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,7 +280,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,10 +312,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -347,7 +346,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -523,14 +521,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
@@ -538,7 +536,7 @@
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -552,7 +550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -573,20 +571,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -594,7 +592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -609,14 +607,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
@@ -624,7 +622,7 @@
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -635,7 +633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -653,24 +651,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -681,14 +679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
@@ -696,7 +694,7 @@
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -710,7 +708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -731,14 +729,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
@@ -748,7 +746,7 @@
     <col min="6" max="6" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -759,7 +757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -776,14 +774,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
@@ -796,7 +794,7 @@
     <col min="9" max="9" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -825,7 +823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -841,7 +839,7 @@
       <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="11" t="s">
         <v>38</v>
       </c>
       <c r="G2" s="1" t="s">

</xml_diff>